<commit_message>
feat: Enhance budget reader and merge functions; add output handling and logging
</commit_message>
<xml_diff>
--- a/data/inputs/saude_esteira/BASE_LISTA_UPES_DOCUMENTS.xlsx
+++ b/data/inputs/saude_esteira/BASE_LISTA_UPES_DOCUMENTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/inputs/saude_esteira/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CF1ED65-4AF9-4CE3-9FB7-12FC109E98B5}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2730EBE3-77B2-4E0F-B54C-6DE3A4B502D9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,6 +150,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,7 +422,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,11 +440,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>188292</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>105424</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>